<commit_message>
added excel sheet. automation code for homepage.
</commit_message>
<xml_diff>
--- a/ecodersCRM_project_Group/Manual_Documents/CRM_Saranya.xlsx
+++ b/ecodersCRM_project_Group/Manual_Documents/CRM_Saranya.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\Desktop\saranya_ecoderrs_crm_project_automation\Ecoders_CRM\ecodersCRM_project_Group\Manual_Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10070" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="10068" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test_Scenario" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="119">
   <si>
     <t>Test Scenario</t>
   </si>
@@ -382,6 +382,9 @@
   </si>
   <si>
     <t>User clicks on Dashboard link/tab, Admins dashboard page should be displayed</t>
+  </si>
+  <si>
+    <t>CRM_TC_01</t>
   </si>
 </sst>
 </file>
@@ -788,21 +791,21 @@
       <selection activeCell="B8" sqref="B8:C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.6328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="180.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="3"/>
+    <col min="1" max="1" width="5.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="180.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.77734375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>67</v>
       </c>
@@ -813,7 +816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -827,7 +830,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>2</v>
       </c>
@@ -838,7 +841,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>3</v>
       </c>
@@ -849,7 +852,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>4</v>
       </c>
@@ -860,7 +863,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>5</v>
       </c>
@@ -871,7 +874,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>6</v>
       </c>
@@ -882,7 +885,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>7</v>
       </c>
@@ -893,7 +896,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>8</v>
       </c>
@@ -904,7 +907,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>9</v>
       </c>
@@ -915,7 +918,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>10</v>
       </c>
@@ -926,7 +929,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>11</v>
       </c>
@@ -937,7 +940,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>12</v>
       </c>
@@ -948,7 +951,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>13</v>
       </c>
@@ -959,7 +962,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>14</v>
       </c>
@@ -970,7 +973,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>15</v>
       </c>
@@ -981,7 +984,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>16</v>
       </c>
@@ -992,7 +995,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>17</v>
       </c>
@@ -1003,7 +1006,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>18</v>
       </c>
@@ -1014,7 +1017,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>19</v>
       </c>
@@ -1025,7 +1028,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>20</v>
       </c>
@@ -1036,7 +1039,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="31" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>21</v>
       </c>
@@ -1047,7 +1050,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>22</v>
       </c>
@@ -1058,7 +1061,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>23</v>
       </c>
@@ -1069,7 +1072,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>24</v>
       </c>
@@ -1080,7 +1083,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>25</v>
       </c>
@@ -1091,7 +1094,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>26</v>
       </c>
@@ -1102,7 +1105,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>27</v>
       </c>
@@ -1113,7 +1116,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>28</v>
       </c>
@@ -1124,7 +1127,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>29</v>
       </c>
@@ -1135,7 +1138,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>30</v>
       </c>
@@ -1146,7 +1149,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>31</v>
       </c>
@@ -1157,7 +1160,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>32</v>
       </c>
@@ -1178,28 +1181,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="C110" sqref="C110"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.26953125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.54296875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="183.7265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.26953125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.1796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="183.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.21875" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="42" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.36328125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="6"/>
+    <col min="7" max="7" width="6.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.77734375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>69</v>
       </c>
@@ -1213,7 +1216,7 @@
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
     </row>
-    <row r="4" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1233,7 +1236,7 @@
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
     </row>
-    <row r="5" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5"/>
       <c r="B5" s="3" t="s">
         <v>13</v>
@@ -1247,7 +1250,7 @@
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
     </row>
-    <row r="6" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
@@ -1257,7 +1260,7 @@
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
     </row>
-    <row r="7" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -1267,7 +1270,7 @@
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
     </row>
-    <row r="8" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -1277,7 +1280,7 @@
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
     </row>
-    <row r="9" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9"/>
       <c r="B9" s="8" t="s">
         <v>74</v>
@@ -1289,13 +1292,13 @@
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
     </row>
-    <row r="10" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10"/>
       <c r="B10" s="9" t="s">
         <v>75</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>13</v>
+        <v>118</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
@@ -1303,7 +1306,7 @@
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
     </row>
-    <row r="11" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11"/>
       <c r="B11" s="9" t="s">
         <v>76</v>
@@ -1317,7 +1320,7 @@
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
     </row>
-    <row r="12" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12"/>
       <c r="B12" s="9" t="s">
         <v>77</v>
@@ -1331,7 +1334,7 @@
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
     </row>
-    <row r="13" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13"/>
       <c r="B13" s="9" t="s">
         <v>78</v>
@@ -1345,7 +1348,7 @@
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
     </row>
-    <row r="14" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14"/>
       <c r="B14" s="9" t="s">
         <v>79</v>
@@ -1359,7 +1362,7 @@
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
     </row>
-    <row r="15" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15"/>
       <c r="B15" s="9" t="s">
         <v>81</v>
@@ -1373,7 +1376,7 @@
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
     </row>
-    <row r="16" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16"/>
       <c r="B16" s="9" t="s">
         <v>82</v>
@@ -1387,7 +1390,7 @@
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
     </row>
-    <row r="17" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17"/>
       <c r="B17" s="9" t="s">
         <v>84</v>
@@ -1401,7 +1404,7 @@
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
     </row>
-    <row r="18" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18"/>
       <c r="B18" s="9" t="s">
         <v>85</v>
@@ -1415,7 +1418,7 @@
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
     </row>
-    <row r="19" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19"/>
       <c r="B19" s="9" t="s">
         <v>86</v>
@@ -1429,7 +1432,7 @@
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
     </row>
-    <row r="20" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20"/>
       <c r="B20" s="9" t="s">
         <v>87</v>
@@ -1441,7 +1444,7 @@
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
     </row>
-    <row r="21" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -1451,7 +1454,7 @@
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
     </row>
-    <row r="22" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22"/>
       <c r="B22" s="8" t="s">
         <v>88</v>
@@ -1463,7 +1466,7 @@
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
     </row>
-    <row r="23" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A23"/>
       <c r="B23" s="8" t="s">
         <v>89</v>
@@ -1487,7 +1490,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A24"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -1497,7 +1500,7 @@
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
     </row>
-    <row r="25" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A25"/>
       <c r="B25" s="9">
         <v>1</v>
@@ -1519,7 +1522,7 @@
       </c>
       <c r="H25" s="9"/>
     </row>
-    <row r="26" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A26"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
@@ -1529,7 +1532,7 @@
       <c r="G26" s="9"/>
       <c r="H26" s="9"/>
     </row>
-    <row r="27" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A27"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -1539,7 +1542,7 @@
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
     </row>
-    <row r="28" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A28"/>
       <c r="B28" s="8" t="s">
         <v>97</v>
@@ -1553,7 +1556,7 @@
       <c r="G28" s="9"/>
       <c r="H28" s="9"/>
     </row>
-    <row r="29" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A29"/>
       <c r="B29" s="8" t="s">
         <v>99</v>
@@ -1567,7 +1570,7 @@
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
     </row>
-    <row r="30" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A30"/>
       <c r="B30" s="8" t="s">
         <v>101</v>
@@ -1581,7 +1584,7 @@
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
     </row>
-    <row r="31" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A31"/>
       <c r="B31" s="8" t="s">
         <v>102</v>
@@ -1593,7 +1596,7 @@
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
     </row>
-    <row r="32" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A32"/>
       <c r="B32" s="8"/>
       <c r="C32" s="12"/>
@@ -1603,7 +1606,7 @@
       <c r="G32" s="9"/>
       <c r="H32" s="9"/>
     </row>
-    <row r="33" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2</v>
       </c>
@@ -1623,7 +1626,7 @@
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
     </row>
-    <row r="34" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34"/>
       <c r="B34" s="3" t="s">
         <v>14</v>
@@ -1637,7 +1640,7 @@
       <c r="G34" s="9"/>
       <c r="H34" s="9"/>
     </row>
-    <row r="35" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A35"/>
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>
@@ -1647,7 +1650,7 @@
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
     </row>
-    <row r="36" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A36"/>
       <c r="B36" s="8" t="s">
         <v>74</v>
@@ -1659,7 +1662,7 @@
       <c r="G36" s="9"/>
       <c r="H36" s="9"/>
     </row>
-    <row r="37" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37"/>
       <c r="B37" s="9" t="s">
         <v>75</v>
@@ -1673,7 +1676,7 @@
       <c r="G37" s="9"/>
       <c r="H37" s="9"/>
     </row>
-    <row r="38" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A38"/>
       <c r="B38" s="9" t="s">
         <v>76</v>
@@ -1687,7 +1690,7 @@
       <c r="G38" s="9"/>
       <c r="H38" s="9"/>
     </row>
-    <row r="39" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A39"/>
       <c r="B39" s="9" t="s">
         <v>77</v>
@@ -1701,7 +1704,7 @@
       <c r="G39" s="9"/>
       <c r="H39" s="9"/>
     </row>
-    <row r="40" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A40"/>
       <c r="B40" s="9" t="s">
         <v>78</v>
@@ -1715,7 +1718,7 @@
       <c r="G40" s="9"/>
       <c r="H40" s="9"/>
     </row>
-    <row r="41" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A41"/>
       <c r="B41" s="9" t="s">
         <v>79</v>
@@ -1729,7 +1732,7 @@
       <c r="G41" s="9"/>
       <c r="H41" s="9"/>
     </row>
-    <row r="42" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A42"/>
       <c r="B42" s="9" t="s">
         <v>81</v>
@@ -1743,7 +1746,7 @@
       <c r="G42" s="9"/>
       <c r="H42" s="9"/>
     </row>
-    <row r="43" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A43"/>
       <c r="B43" s="9" t="s">
         <v>82</v>
@@ -1757,7 +1760,7 @@
       <c r="G43" s="9"/>
       <c r="H43" s="9"/>
     </row>
-    <row r="44" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A44"/>
       <c r="B44" s="9" t="s">
         <v>84</v>
@@ -1771,7 +1774,7 @@
       <c r="G44" s="9"/>
       <c r="H44" s="9"/>
     </row>
-    <row r="45" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A45"/>
       <c r="B45" s="9" t="s">
         <v>85</v>
@@ -1785,7 +1788,7 @@
       <c r="G45" s="9"/>
       <c r="H45" s="9"/>
     </row>
-    <row r="46" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A46"/>
       <c r="B46" s="9" t="s">
         <v>86</v>
@@ -1799,7 +1802,7 @@
       <c r="G46" s="9"/>
       <c r="H46" s="9"/>
     </row>
-    <row r="47" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A47"/>
       <c r="B47" s="9" t="s">
         <v>87</v>
@@ -1811,7 +1814,7 @@
       <c r="G47" s="9"/>
       <c r="H47" s="9"/>
     </row>
-    <row r="48" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A48"/>
       <c r="B48" s="9"/>
       <c r="C48" s="9"/>
@@ -1821,7 +1824,7 @@
       <c r="G48" s="9"/>
       <c r="H48" s="9"/>
     </row>
-    <row r="49" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A49"/>
       <c r="B49" s="8" t="s">
         <v>88</v>
@@ -1833,7 +1836,7 @@
       <c r="G49" s="8"/>
       <c r="H49" s="8"/>
     </row>
-    <row r="50" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A50"/>
       <c r="B50" s="8" t="s">
         <v>89</v>
@@ -1857,7 +1860,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A51"/>
       <c r="B51" s="9"/>
       <c r="C51" s="9"/>
@@ -1867,7 +1870,7 @@
       <c r="G51" s="9"/>
       <c r="H51" s="9"/>
     </row>
-    <row r="52" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A52"/>
       <c r="B52" s="9">
         <v>1</v>
@@ -1889,7 +1892,7 @@
       </c>
       <c r="H52" s="9"/>
     </row>
-    <row r="53" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A53"/>
       <c r="B53" s="9">
         <v>2</v>
@@ -1911,7 +1914,7 @@
       </c>
       <c r="H53" s="9"/>
     </row>
-    <row r="54" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A54"/>
       <c r="D54" s="9"/>
       <c r="E54" s="9"/>
@@ -1919,7 +1922,7 @@
       <c r="G54" s="9"/>
       <c r="H54" s="9"/>
     </row>
-    <row r="55" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A55"/>
       <c r="B55" s="8" t="s">
         <v>97</v>
@@ -1933,7 +1936,7 @@
       <c r="G55" s="9"/>
       <c r="H55" s="9"/>
     </row>
-    <row r="56" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A56"/>
       <c r="B56" s="8" t="s">
         <v>99</v>
@@ -1947,7 +1950,7 @@
       <c r="G56" s="9"/>
       <c r="H56" s="9"/>
     </row>
-    <row r="57" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A57"/>
       <c r="B57" s="8" t="s">
         <v>101</v>
@@ -1961,7 +1964,7 @@
       <c r="G57" s="9"/>
       <c r="H57" s="9"/>
     </row>
-    <row r="58" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A58"/>
       <c r="B58" s="8" t="s">
         <v>102</v>
@@ -1973,10 +1976,10 @@
       <c r="G58" s="9"/>
       <c r="H58" s="9"/>
     </row>
-    <row r="59" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A59"/>
     </row>
-    <row r="60" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>3</v>
       </c>
@@ -1996,7 +1999,7 @@
       <c r="G60" s="9"/>
       <c r="H60" s="9"/>
     </row>
-    <row r="61" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61"/>
       <c r="B61" s="3" t="s">
         <v>15</v>
@@ -2010,7 +2013,7 @@
       <c r="G61" s="9"/>
       <c r="H61" s="9"/>
     </row>
-    <row r="62" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A62"/>
       <c r="B62" s="9"/>
       <c r="C62" s="9"/>
@@ -2020,7 +2023,7 @@
       <c r="G62" s="9"/>
       <c r="H62" s="9"/>
     </row>
-    <row r="63" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A63"/>
       <c r="B63" s="8" t="s">
         <v>74</v>
@@ -2032,7 +2035,7 @@
       <c r="G63" s="9"/>
       <c r="H63" s="9"/>
     </row>
-    <row r="64" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A64"/>
       <c r="B64" s="9" t="s">
         <v>75</v>
@@ -2046,7 +2049,7 @@
       <c r="G64" s="9"/>
       <c r="H64" s="9"/>
     </row>
-    <row r="65" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A65"/>
       <c r="B65" s="9" t="s">
         <v>76</v>
@@ -2060,7 +2063,7 @@
       <c r="G65" s="9"/>
       <c r="H65" s="9"/>
     </row>
-    <row r="66" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A66"/>
       <c r="B66" s="9" t="s">
         <v>77</v>
@@ -2074,7 +2077,7 @@
       <c r="G66" s="9"/>
       <c r="H66" s="9"/>
     </row>
-    <row r="67" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A67"/>
       <c r="B67" s="9" t="s">
         <v>78</v>
@@ -2088,7 +2091,7 @@
       <c r="G67" s="9"/>
       <c r="H67" s="9"/>
     </row>
-    <row r="68" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A68"/>
       <c r="B68" s="9" t="s">
         <v>79</v>
@@ -2102,7 +2105,7 @@
       <c r="G68" s="9"/>
       <c r="H68" s="9"/>
     </row>
-    <row r="69" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A69"/>
       <c r="B69" s="9" t="s">
         <v>81</v>
@@ -2116,7 +2119,7 @@
       <c r="G69" s="9"/>
       <c r="H69" s="9"/>
     </row>
-    <row r="70" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A70"/>
       <c r="B70" s="9" t="s">
         <v>82</v>
@@ -2130,7 +2133,7 @@
       <c r="G70" s="9"/>
       <c r="H70" s="9"/>
     </row>
-    <row r="71" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A71"/>
       <c r="B71" s="9" t="s">
         <v>84</v>
@@ -2144,7 +2147,7 @@
       <c r="G71" s="9"/>
       <c r="H71" s="9"/>
     </row>
-    <row r="72" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A72"/>
       <c r="B72" s="9" t="s">
         <v>85</v>
@@ -2158,7 +2161,7 @@
       <c r="G72" s="9"/>
       <c r="H72" s="9"/>
     </row>
-    <row r="73" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A73"/>
       <c r="B73" s="9" t="s">
         <v>86</v>
@@ -2172,7 +2175,7 @@
       <c r="G73" s="9"/>
       <c r="H73" s="9"/>
     </row>
-    <row r="74" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A74"/>
       <c r="B74" s="9" t="s">
         <v>87</v>
@@ -2184,7 +2187,7 @@
       <c r="G74" s="9"/>
       <c r="H74" s="9"/>
     </row>
-    <row r="75" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A75"/>
       <c r="B75" s="9"/>
       <c r="C75" s="9"/>
@@ -2194,7 +2197,7 @@
       <c r="G75" s="9"/>
       <c r="H75" s="9"/>
     </row>
-    <row r="76" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A76"/>
       <c r="B76" s="8" t="s">
         <v>88</v>
@@ -2206,7 +2209,7 @@
       <c r="G76" s="8"/>
       <c r="H76" s="8"/>
     </row>
-    <row r="77" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A77"/>
       <c r="B77" s="8" t="s">
         <v>89</v>
@@ -2230,7 +2233,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A78"/>
       <c r="B78" s="9"/>
       <c r="C78" s="9"/>
@@ -2240,7 +2243,7 @@
       <c r="G78" s="9"/>
       <c r="H78" s="9"/>
     </row>
-    <row r="79" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A79"/>
       <c r="B79" s="9">
         <v>1</v>
@@ -2262,7 +2265,7 @@
       </c>
       <c r="H79" s="9"/>
     </row>
-    <row r="80" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A80"/>
       <c r="B80" s="9">
         <v>2</v>
@@ -2284,7 +2287,7 @@
       </c>
       <c r="H80" s="9"/>
     </row>
-    <row r="81" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A81"/>
       <c r="D81" s="9"/>
       <c r="E81" s="9"/>
@@ -2292,7 +2295,7 @@
       <c r="G81" s="9"/>
       <c r="H81" s="9"/>
     </row>
-    <row r="82" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A82"/>
       <c r="B82" s="8" t="s">
         <v>97</v>
@@ -2306,7 +2309,7 @@
       <c r="G82" s="9"/>
       <c r="H82" s="9"/>
     </row>
-    <row r="83" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A83"/>
       <c r="B83" s="8" t="s">
         <v>99</v>
@@ -2320,7 +2323,7 @@
       <c r="G83" s="9"/>
       <c r="H83" s="9"/>
     </row>
-    <row r="84" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A84"/>
       <c r="B84" s="8" t="s">
         <v>101</v>
@@ -2334,7 +2337,7 @@
       <c r="G84" s="9"/>
       <c r="H84" s="9"/>
     </row>
-    <row r="85" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A85"/>
       <c r="B85" s="8" t="s">
         <v>102</v>
@@ -2346,7 +2349,7 @@
       <c r="G85" s="9"/>
       <c r="H85" s="9"/>
     </row>
-    <row r="86" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A86"/>
       <c r="B86" s="8"/>
       <c r="C86" s="9"/>
@@ -2356,7 +2359,7 @@
       <c r="G86" s="9"/>
       <c r="H86" s="9"/>
     </row>
-    <row r="87" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>4</v>
       </c>
@@ -2376,7 +2379,7 @@
       <c r="G87" s="9"/>
       <c r="H87" s="9"/>
     </row>
-    <row r="88" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A88"/>
       <c r="B88" s="3" t="s">
         <v>16</v>
@@ -2390,7 +2393,7 @@
       <c r="G88" s="9"/>
       <c r="H88" s="9"/>
     </row>
-    <row r="89" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A89"/>
       <c r="B89" s="9"/>
       <c r="C89" s="9"/>
@@ -2400,7 +2403,7 @@
       <c r="G89" s="9"/>
       <c r="H89" s="9"/>
     </row>
-    <row r="90" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A90"/>
       <c r="B90" s="8" t="s">
         <v>74</v>
@@ -2412,7 +2415,7 @@
       <c r="G90" s="9"/>
       <c r="H90" s="9"/>
     </row>
-    <row r="91" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A91"/>
       <c r="B91" s="9" t="s">
         <v>75</v>
@@ -2426,7 +2429,7 @@
       <c r="G91" s="9"/>
       <c r="H91" s="9"/>
     </row>
-    <row r="92" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A92"/>
       <c r="B92" s="9" t="s">
         <v>76</v>
@@ -2440,7 +2443,7 @@
       <c r="G92" s="9"/>
       <c r="H92" s="9"/>
     </row>
-    <row r="93" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A93"/>
       <c r="B93" s="9" t="s">
         <v>77</v>
@@ -2454,7 +2457,7 @@
       <c r="G93" s="9"/>
       <c r="H93" s="9"/>
     </row>
-    <row r="94" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A94"/>
       <c r="B94" s="9" t="s">
         <v>78</v>
@@ -2468,7 +2471,7 @@
       <c r="G94" s="9"/>
       <c r="H94" s="9"/>
     </row>
-    <row r="95" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A95"/>
       <c r="B95" s="9" t="s">
         <v>79</v>
@@ -2482,7 +2485,7 @@
       <c r="G95" s="9"/>
       <c r="H95" s="9"/>
     </row>
-    <row r="96" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A96"/>
       <c r="B96" s="9" t="s">
         <v>81</v>
@@ -2496,7 +2499,7 @@
       <c r="G96" s="9"/>
       <c r="H96" s="9"/>
     </row>
-    <row r="97" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A97"/>
       <c r="B97" s="9" t="s">
         <v>82</v>
@@ -2510,7 +2513,7 @@
       <c r="G97" s="9"/>
       <c r="H97" s="9"/>
     </row>
-    <row r="98" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A98"/>
       <c r="B98" s="9" t="s">
         <v>84</v>
@@ -2524,7 +2527,7 @@
       <c r="G98" s="9"/>
       <c r="H98" s="9"/>
     </row>
-    <row r="99" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A99"/>
       <c r="B99" s="9" t="s">
         <v>85</v>
@@ -2538,7 +2541,7 @@
       <c r="G99" s="9"/>
       <c r="H99" s="9"/>
     </row>
-    <row r="100" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A100"/>
       <c r="B100" s="9" t="s">
         <v>86</v>
@@ -2552,7 +2555,7 @@
       <c r="G100" s="9"/>
       <c r="H100" s="9"/>
     </row>
-    <row r="101" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A101"/>
       <c r="B101" s="9" t="s">
         <v>87</v>
@@ -2564,7 +2567,7 @@
       <c r="G101" s="9"/>
       <c r="H101" s="9"/>
     </row>
-    <row r="102" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A102"/>
       <c r="B102" s="9"/>
       <c r="C102" s="9"/>
@@ -2574,7 +2577,7 @@
       <c r="G102" s="9"/>
       <c r="H102" s="9"/>
     </row>
-    <row r="103" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A103"/>
       <c r="B103" s="8" t="s">
         <v>88</v>
@@ -2586,7 +2589,7 @@
       <c r="G103" s="8"/>
       <c r="H103" s="8"/>
     </row>
-    <row r="104" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A104"/>
       <c r="B104" s="8" t="s">
         <v>89</v>
@@ -2610,7 +2613,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A105"/>
       <c r="B105" s="9"/>
       <c r="C105" s="9"/>
@@ -2620,7 +2623,7 @@
       <c r="G105" s="9"/>
       <c r="H105" s="9"/>
     </row>
-    <row r="106" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A106"/>
       <c r="B106" s="9">
         <v>1</v>
@@ -2642,7 +2645,7 @@
       </c>
       <c r="H106" s="9"/>
     </row>
-    <row r="107" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A107"/>
       <c r="B107" s="9">
         <v>2</v>
@@ -2664,7 +2667,7 @@
       </c>
       <c r="H107" s="9"/>
     </row>
-    <row r="108" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A108"/>
       <c r="D108" s="9"/>
       <c r="E108" s="9"/>
@@ -2672,7 +2675,7 @@
       <c r="G108" s="9"/>
       <c r="H108" s="9"/>
     </row>
-    <row r="109" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A109"/>
       <c r="B109" s="8" t="s">
         <v>97</v>
@@ -2686,7 +2689,7 @@
       <c r="G109" s="9"/>
       <c r="H109" s="9"/>
     </row>
-    <row r="110" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A110"/>
       <c r="B110" s="8" t="s">
         <v>99</v>
@@ -2700,7 +2703,7 @@
       <c r="G110" s="9"/>
       <c r="H110" s="9"/>
     </row>
-    <row r="111" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A111"/>
       <c r="B111" s="8" t="s">
         <v>101</v>
@@ -2714,7 +2717,7 @@
       <c r="G111" s="9"/>
       <c r="H111" s="9"/>
     </row>
-    <row r="112" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A112"/>
       <c r="B112" s="8" t="s">
         <v>102</v>
@@ -2726,7 +2729,7 @@
       <c r="G112" s="9"/>
       <c r="H112" s="9"/>
     </row>
-    <row r="113" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A113"/>
       <c r="B113" s="9"/>
       <c r="C113" s="9"/>
@@ -2736,7 +2739,7 @@
       <c r="G113" s="9"/>
       <c r="H113" s="9"/>
     </row>
-    <row r="114" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A114" s="1"/>
       <c r="B114" s="9"/>
       <c r="C114" s="9"/>
@@ -2746,7 +2749,7 @@
       <c r="G114" s="9"/>
       <c r="H114" s="9"/>
     </row>
-    <row r="115" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A115"/>
       <c r="B115" s="8"/>
       <c r="C115" s="9"/>
@@ -2756,7 +2759,7 @@
       <c r="G115" s="9"/>
       <c r="H115" s="9"/>
     </row>
-    <row r="116" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A116"/>
       <c r="B116" s="8"/>
       <c r="C116" s="9"/>
@@ -2766,7 +2769,7 @@
       <c r="G116" s="9"/>
       <c r="H116" s="9"/>
     </row>
-    <row r="117" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A117"/>
       <c r="B117" s="8"/>
       <c r="C117" s="9"/>
@@ -2776,7 +2779,7 @@
       <c r="G117" s="9"/>
       <c r="H117" s="9"/>
     </row>
-    <row r="118" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A118"/>
       <c r="B118" s="8"/>
       <c r="C118" s="12"/>
@@ -2786,7 +2789,7 @@
       <c r="G118" s="9"/>
       <c r="H118" s="9"/>
     </row>
-    <row r="120" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A120"/>
       <c r="B120" s="8"/>
       <c r="C120" s="8"/>
@@ -2796,7 +2799,7 @@
       <c r="G120" s="9"/>
       <c r="H120" s="9"/>
     </row>
-    <row r="121" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A121"/>
       <c r="B121" s="3"/>
       <c r="C121" s="4"/>
@@ -2806,7 +2809,7 @@
       <c r="G121" s="9"/>
       <c r="H121" s="9"/>
     </row>
-    <row r="122" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A122"/>
       <c r="B122" s="9"/>
       <c r="C122" s="9"/>
@@ -2816,7 +2819,7 @@
       <c r="G122" s="9"/>
       <c r="H122" s="9"/>
     </row>
-    <row r="123" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A123"/>
       <c r="B123" s="9"/>
       <c r="C123" s="9"/>
@@ -2826,7 +2829,7 @@
       <c r="G123" s="9"/>
       <c r="H123" s="9"/>
     </row>
-    <row r="124" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A124"/>
       <c r="B124" s="9"/>
       <c r="C124" s="9"/>
@@ -2836,7 +2839,7 @@
       <c r="G124" s="9"/>
       <c r="H124" s="9"/>
     </row>
-    <row r="125" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A125"/>
       <c r="B125" s="8"/>
       <c r="C125" s="9"/>
@@ -2846,7 +2849,7 @@
       <c r="G125" s="9"/>
       <c r="H125" s="9"/>
     </row>
-    <row r="126" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A126"/>
       <c r="B126" s="9"/>
       <c r="C126" s="3"/>
@@ -2856,7 +2859,7 @@
       <c r="G126" s="9"/>
       <c r="H126" s="9"/>
     </row>
-    <row r="127" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A127"/>
       <c r="B127" s="9"/>
       <c r="C127" s="9"/>
@@ -2866,7 +2869,7 @@
       <c r="G127" s="9"/>
       <c r="H127" s="9"/>
     </row>
-    <row r="128" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A128"/>
       <c r="B128" s="9"/>
       <c r="C128" s="10"/>
@@ -2876,7 +2879,7 @@
       <c r="G128" s="9"/>
       <c r="H128" s="9"/>
     </row>
-    <row r="129" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A129"/>
       <c r="B129" s="9"/>
       <c r="C129" s="9"/>
@@ -2886,7 +2889,7 @@
       <c r="G129" s="9"/>
       <c r="H129" s="9"/>
     </row>
-    <row r="130" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A130"/>
       <c r="B130" s="9"/>
       <c r="C130" s="9"/>
@@ -2896,7 +2899,7 @@
       <c r="G130" s="9"/>
       <c r="H130" s="9"/>
     </row>
-    <row r="131" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A131"/>
       <c r="B131" s="9"/>
       <c r="C131" s="11"/>
@@ -2906,7 +2909,7 @@
       <c r="G131" s="9"/>
       <c r="H131" s="9"/>
     </row>
-    <row r="132" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A132"/>
       <c r="B132" s="9"/>
       <c r="C132" s="9"/>
@@ -2916,7 +2919,7 @@
       <c r="G132" s="9"/>
       <c r="H132" s="9"/>
     </row>
-    <row r="133" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A133"/>
       <c r="B133" s="9"/>
       <c r="C133" s="9"/>
@@ -2926,7 +2929,7 @@
       <c r="G133" s="9"/>
       <c r="H133" s="9"/>
     </row>
-    <row r="134" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A134"/>
       <c r="B134" s="9"/>
       <c r="C134" s="9"/>
@@ -2936,7 +2939,7 @@
       <c r="G134" s="9"/>
       <c r="H134" s="9"/>
     </row>
-    <row r="135" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A135"/>
       <c r="B135" s="9"/>
       <c r="C135" s="9"/>
@@ -2946,7 +2949,7 @@
       <c r="G135" s="9"/>
       <c r="H135" s="9"/>
     </row>
-    <row r="136" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A136"/>
       <c r="B136" s="9"/>
       <c r="C136" s="9"/>
@@ -2956,7 +2959,7 @@
       <c r="G136" s="9"/>
       <c r="H136" s="9"/>
     </row>
-    <row r="137" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A137"/>
       <c r="B137" s="9"/>
       <c r="C137" s="9"/>
@@ -2966,7 +2969,7 @@
       <c r="G137" s="9"/>
       <c r="H137" s="9"/>
     </row>
-    <row r="138" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A138"/>
       <c r="B138" s="8"/>
       <c r="C138" s="8"/>
@@ -2976,7 +2979,7 @@
       <c r="G138" s="8"/>
       <c r="H138" s="8"/>
     </row>
-    <row r="139" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A139"/>
       <c r="B139" s="8"/>
       <c r="C139" s="8"/>
@@ -2992,7 +2995,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="140" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A140"/>
       <c r="B140" s="9"/>
       <c r="C140" s="9"/>
@@ -3002,7 +3005,7 @@
       <c r="G140" s="9"/>
       <c r="H140" s="9"/>
     </row>
-    <row r="141" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A141"/>
       <c r="B141" s="9"/>
       <c r="C141" s="9"/>
@@ -3016,7 +3019,7 @@
       </c>
       <c r="H141" s="9"/>
     </row>
-    <row r="142" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A142"/>
       <c r="B142" s="9"/>
       <c r="C142" s="9"/>
@@ -3026,7 +3029,7 @@
       <c r="G142" s="9"/>
       <c r="H142" s="9"/>
     </row>
-    <row r="143" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A143"/>
       <c r="B143" s="9"/>
       <c r="C143" s="9"/>
@@ -3036,7 +3039,7 @@
       <c r="G143" s="9"/>
       <c r="H143" s="9"/>
     </row>
-    <row r="144" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A144"/>
       <c r="B144" s="8"/>
       <c r="C144" s="9"/>
@@ -3046,7 +3049,7 @@
       <c r="G144" s="9"/>
       <c r="H144" s="9"/>
     </row>
-    <row r="145" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A145"/>
       <c r="B145" s="8"/>
       <c r="C145" s="9"/>
@@ -3056,7 +3059,7 @@
       <c r="G145" s="9"/>
       <c r="H145" s="9"/>
     </row>
-    <row r="146" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A146"/>
       <c r="B146" s="8"/>
       <c r="C146" s="9"/>
@@ -3066,7 +3069,7 @@
       <c r="G146" s="9"/>
       <c r="H146" s="9"/>
     </row>
-    <row r="147" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A147"/>
       <c r="B147" s="8"/>
       <c r="C147" s="12"/>
@@ -3098,7 +3101,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3112,10 +3115,10 @@
       <selection activeCell="B5" sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>